<commit_message>
Commit use case detail
</commit_message>
<xml_diff>
--- a/document/diagram/use_case/UseCase.xlsx
+++ b/document/diagram/use_case/UseCase.xlsx
@@ -638,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1094,20 +1094,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27">
+    <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="1">
         <v>11</v>
       </c>
     </row>

</xml_diff>